<commit_message>
Changes regarding javascript functionality in script
Signed-off-by: Love Mishra <lovemishrahdr@gmail.com>
</commit_message>
<xml_diff>
--- a/datafiles/google.xlsx
+++ b/datafiles/google.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/love.mishra/git/excelkeyword/framework/testingframework/hybrid/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BAD9E1-F7B4-8945-8685-3715F6024B62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880DBBF7-9DBA-B64C-A51B-BF6D26625BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Firefox Driver Capabilities
Signed-off-by: Love Mishra <lovemishrahdr@gmail.com>
</commit_message>
<xml_diff>
--- a/datafiles/google.xlsx
+++ b/datafiles/google.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/love.mishra/git/excelkeyword/framework/testingframework/hybrid/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7270E75A-98FE-A146-872F-3777728040A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF375E24-7673-C24C-820E-38C7E1F70DAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Love Mishra</t>
   </si>
   <si>
-    <t>Pause the script for 5 sec</t>
-  </si>
-  <si>
     <t>TC_002</t>
   </si>
   <si>
@@ -128,13 +125,34 @@
     <t>Verify text on element</t>
   </si>
   <si>
-    <t>elementcontainstext</t>
-  </si>
-  <si>
     <t>(//legend)[1]</t>
   </si>
   <si>
     <t>Radio Button Example</t>
+  </si>
+  <si>
+    <t>Navigate</t>
+  </si>
+  <si>
+    <t>https://www.selenium.dev/downloads/</t>
+  </si>
+  <si>
+    <t>Navigate to selenium download</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>Download jar file</t>
+  </si>
+  <si>
+    <t>//p[contains(text(),'Latest stable version')]//a[contains(text(),'3.141.59')]</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>ElementContainsText</t>
   </si>
 </sst>
 </file>
@@ -577,21 +595,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E6435A-4A30-1E40-B69D-13C9C3479EA8}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -626,43 +644,43 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -683,7 +701,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -704,7 +722,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -725,7 +743,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -734,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>7</v>
@@ -748,25 +766,68 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3">
-        <v>5</v>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{35C0CBC1-BA88-CA4D-B01A-89E33879BA77}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>